<commit_message>
Add flask-uploads for gallery :astonished:
</commit_message>
<xml_diff>
--- a/installed_packages_to_markdown.xlsx
+++ b/installed_packages_to_markdown.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Step 1. Run the comand line below.</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Flask==1.0.2</t>
+  </si>
+  <si>
+    <t>Flask-Uploads==0.2.1</t>
   </si>
   <si>
     <t>isort==4.3.4</t>
@@ -119,10 +122,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -184,14 +187,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -199,9 +194,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,6 +209,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -225,29 +234,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,25 +256,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -293,14 +295,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -320,13 +330,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -349,187 +352,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,6 +607,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -626,21 +644,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -682,152 +685,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -868,12 +871,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1238,7 +1235,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1275,7 +1272,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
-      <c r="H2" s="16"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" ht="21" customHeight="1" spans="1:8">
       <c r="A3" s="10" t="s">
@@ -1308,7 +1305,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="13"/>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1319,898 +1316,901 @@
         <v>6</v>
       </c>
       <c r="D6" s="13"/>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="15" t="str">
+      <c r="C7" s="4" t="str">
         <f>IF(A7="","",CONCATENATE("| ",SUBSTITUTE(A7,"=="," | ")," |"))</f>
         <v>| astroid | 2.1.0 |</v>
       </c>
-      <c r="E7" s="18" t="str">
+      <c r="E7" s="16" t="str">
         <f t="shared" ref="E7:E70" si="0">IF(C7="","",SUBSTITUTE(MID(C7,3,LEN(C7)-4)," | ",","))</f>
         <v>astroid,2.1.0</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="15" t="str">
+      <c r="C8" s="4" t="str">
         <f t="shared" ref="C8:C39" si="1">IF(A8="","",CONCATENATE("| ",SUBSTITUTE(A8,"=="," | ")," |"))</f>
         <v>| Click | 7.0 |</v>
       </c>
-      <c r="E8" s="18" t="str">
+      <c r="E8" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Click,7.0</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="15" t="str">
+      <c r="C9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| et-xmlfile | 1.0.1 |</v>
       </c>
-      <c r="E9" s="18" t="str">
+      <c r="E9" s="16" t="str">
         <f t="shared" si="0"/>
         <v>et-xmlfile,1.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="15" t="str">
+      <c r="C10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| Flask | 1.0.2 |</v>
       </c>
-      <c r="E10" s="18" t="str">
+      <c r="E10" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Flask,1.0.2</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="15" t="str">
+      <c r="C11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| Flask-Uploads | 0.2.1 |</v>
+      </c>
+      <c r="E11" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>Flask-Uploads,0.2.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| isort | 4.3.4 |</v>
       </c>
-      <c r="E11" s="18" t="str">
+      <c r="E12" s="16" t="str">
         <f t="shared" si="0"/>
         <v>isort,4.3.4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="15" t="str">
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| itsdangerous | 1.1.0 |</v>
       </c>
-      <c r="E12" s="18" t="str">
+      <c r="E13" s="16" t="str">
         <f t="shared" si="0"/>
         <v>itsdangerous,1.1.0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="15" t="str">
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| jdcal | 1.4 |</v>
       </c>
-      <c r="E13" s="18" t="str">
+      <c r="E14" s="16" t="str">
         <f t="shared" si="0"/>
         <v>jdcal,1.4</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="15" t="str">
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| Jinja2 | 2.10 |</v>
       </c>
-      <c r="E14" s="18" t="str">
+      <c r="E15" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Jinja2,2.10</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="15" t="str">
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| lazy-object-proxy | 1.3.1 |</v>
       </c>
-      <c r="E15" s="18" t="str">
+      <c r="E16" s="16" t="str">
         <f t="shared" si="0"/>
         <v>lazy-object-proxy,1.3.1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="15" t="str">
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| lml | 0.0.9 |</v>
       </c>
-      <c r="E16" s="18" t="str">
+      <c r="E17" s="16" t="str">
         <f t="shared" si="0"/>
         <v>lml,0.0.9</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="15" t="str">
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| Markdown | 3.0.1 |</v>
       </c>
-      <c r="E17" s="18" t="str">
+      <c r="E18" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Markdown,3.0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="15" t="str">
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| MarkupSafe | 1.1.0 |</v>
       </c>
-      <c r="E18" s="18" t="str">
+      <c r="E19" s="16" t="str">
         <f t="shared" si="0"/>
         <v>MarkupSafe,1.1.0</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="15" t="str">
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| mccabe | 0.6.1 |</v>
       </c>
-      <c r="E19" s="18" t="str">
+      <c r="E20" s="16" t="str">
         <f t="shared" si="0"/>
         <v>mccabe,0.6.1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="15" t="str">
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| openpyxl | 2.6.0 |</v>
       </c>
-      <c r="E20" s="18" t="str">
+      <c r="E21" s="16" t="str">
         <f t="shared" si="0"/>
         <v>openpyxl,2.6.0</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="15" t="str">
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| pip | 9.0.1 |</v>
       </c>
-      <c r="E21" s="18" t="str">
+      <c r="E22" s="16" t="str">
         <f t="shared" si="0"/>
         <v>pip,9.0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="15" t="str">
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| pkg-resources | 0.0.0 |</v>
       </c>
-      <c r="E22" s="18" t="str">
+      <c r="E23" s="16" t="str">
         <f t="shared" si="0"/>
         <v>pkg-resources,0.0.0</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="15" t="str">
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| pyexcel-io | 0.5.14 |</v>
       </c>
-      <c r="E23" s="18" t="str">
+      <c r="E24" s="16" t="str">
         <f t="shared" si="0"/>
         <v>pyexcel-io,0.5.14</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="15" t="str">
+    <row r="25" spans="1:5">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| pyexcel-xlsx | 0.5.7 |</v>
       </c>
-      <c r="E24" s="18" t="str">
+      <c r="E25" s="16" t="str">
         <f t="shared" si="0"/>
         <v>pyexcel-xlsx,0.5.7</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="15" t="str">
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| pylint | 2.2.2 |</v>
       </c>
-      <c r="E25" s="18" t="str">
+      <c r="E26" s="16" t="str">
         <f t="shared" si="0"/>
         <v>pylint,2.2.2</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="15" t="str">
+    <row r="27" spans="1:5">
+      <c r="A27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| setuptools | 40.8.0 |</v>
       </c>
-      <c r="E26" s="18" t="str">
+      <c r="E27" s="16" t="str">
         <f t="shared" si="0"/>
         <v>setuptools,40.8.0</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="15" t="str">
+    <row r="28" spans="1:5">
+      <c r="A28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| six | 1.12.0 |</v>
       </c>
-      <c r="E27" s="18" t="str">
+      <c r="E28" s="16" t="str">
         <f t="shared" si="0"/>
         <v>six,1.12.0</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="15" t="str">
+    <row r="29" spans="1:5">
+      <c r="A29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| typed-ast | 1.3.1 |</v>
       </c>
-      <c r="E28" s="18" t="str">
+      <c r="E29" s="16" t="str">
         <f t="shared" si="0"/>
         <v>typed-ast,1.3.1</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="15" t="str">
+    <row r="30" spans="1:5">
+      <c r="A30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| Werkzeug | 0.14.1 |</v>
       </c>
-      <c r="E29" s="18" t="str">
+      <c r="E30" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Werkzeug,0.14.1</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="15" t="str">
+    <row r="31" spans="1:5">
+      <c r="A31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="4" t="str">
         <f t="shared" si="1"/>
         <v>| wrapt | 1.11.1 |</v>
       </c>
-      <c r="E30" s="18" t="str">
+      <c r="E31" s="16" t="str">
         <f t="shared" si="0"/>
         <v>wrapt,1.11.1</v>
       </c>
     </row>
-    <row r="31" spans="3:5">
-      <c r="C31" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E31" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
     <row r="32" spans="3:5">
-      <c r="C32" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E32" s="18" t="str">
+      <c r="C32" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E32" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="33" spans="3:5">
-      <c r="C33" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E33" s="18" t="str">
+      <c r="C33" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E33" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="3:5">
-      <c r="C34" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E34" s="18" t="str">
+      <c r="C34" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E34" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="35" spans="3:5">
-      <c r="C35" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E35" s="18" t="str">
+      <c r="C35" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E35" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="36" spans="3:5">
-      <c r="C36" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E36" s="18" t="str">
+      <c r="C36" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E36" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="3:5">
-      <c r="C37" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E37" s="18" t="str">
+      <c r="C37" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E37" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="3:5">
-      <c r="C38" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E38" s="18" t="str">
+      <c r="C38" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E38" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="3:5">
-      <c r="C39" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E39" s="18" t="str">
+      <c r="C39" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E39" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="3:5">
-      <c r="C40" s="15" t="str">
+      <c r="C40" s="4" t="str">
         <f t="shared" ref="C40:C71" si="2">IF(A40="","",CONCATENATE("| ",SUBSTITUTE(A40,"=="," | ")," |"))</f>
         <v/>
       </c>
-      <c r="E40" s="18" t="str">
+      <c r="E40" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="3:5">
-      <c r="C41" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E41" s="18" t="str">
+      <c r="C41" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E41" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="3:5">
-      <c r="C42" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E42" s="18" t="str">
+      <c r="C42" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E42" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="3:5">
-      <c r="C43" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E43" s="18" t="str">
+      <c r="C43" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E43" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="3:5">
-      <c r="C44" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E44" s="18" t="str">
+      <c r="C44" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E44" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="3:5">
-      <c r="C45" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E45" s="18" t="str">
+      <c r="C45" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E45" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="3:5">
-      <c r="C46" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E46" s="18" t="str">
+      <c r="C46" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E46" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="3:5">
-      <c r="C47" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E47" s="18" t="str">
+      <c r="C47" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E47" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="3:5">
-      <c r="C48" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E48" s="18" t="str">
+      <c r="C48" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E48" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="3:5">
-      <c r="C49" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E49" s="18" t="str">
+      <c r="C49" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E49" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="3:5">
-      <c r="C50" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E50" s="18" t="str">
+      <c r="C50" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E50" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="3:5">
-      <c r="C51" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E51" s="18" t="str">
+      <c r="C51" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E51" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="3:5">
-      <c r="C52" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E52" s="18" t="str">
+      <c r="C52" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E52" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="3:5">
-      <c r="C53" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E53" s="18" t="str">
+      <c r="C53" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E53" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="3:5">
-      <c r="C54" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E54" s="18" t="str">
+      <c r="C54" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E54" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="3:5">
-      <c r="C55" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E55" s="18" t="str">
+      <c r="C55" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E55" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="3:5">
-      <c r="C56" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E56" s="18" t="str">
+      <c r="C56" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E56" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="3:5">
-      <c r="C57" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E57" s="18" t="str">
+      <c r="C57" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E57" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="3:5">
-      <c r="C58" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E58" s="18" t="str">
+      <c r="C58" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E58" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="3:5">
-      <c r="C59" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E59" s="18" t="str">
+      <c r="C59" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E59" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="3:5">
-      <c r="C60" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E60" s="18" t="str">
+      <c r="C60" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E60" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="3:5">
-      <c r="C61" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E61" s="18" t="str">
+      <c r="C61" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E61" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="3:5">
-      <c r="C62" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E62" s="18" t="str">
+      <c r="C62" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E62" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="63" spans="3:5">
-      <c r="C63" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E63" s="18" t="str">
+      <c r="C63" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E63" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="3:5">
-      <c r="C64" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E64" s="18" t="str">
+      <c r="C64" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E64" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="65" spans="3:5">
-      <c r="C65" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E65" s="18" t="str">
+      <c r="C65" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E65" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="66" spans="3:5">
-      <c r="C66" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E66" s="18" t="str">
+      <c r="C66" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E66" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="67" spans="3:5">
-      <c r="C67" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E67" s="18" t="str">
+      <c r="C67" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E67" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="3:5">
-      <c r="C68" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E68" s="18" t="str">
+      <c r="C68" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E68" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="3:5">
-      <c r="C69" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E69" s="18" t="str">
+      <c r="C69" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E69" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="3:5">
-      <c r="C70" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E70" s="18" t="str">
+      <c r="C70" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E70" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="3:5">
-      <c r="C71" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E71" s="18" t="str">
+      <c r="C71" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E71" s="16" t="str">
         <f t="shared" ref="E71:E88" si="3">IF(C71="","",SUBSTITUTE(MID(C71,3,LEN(C71)-4)," | ",","))</f>
         <v/>
       </c>
     </row>
     <row r="72" spans="3:5">
-      <c r="C72" s="15" t="str">
+      <c r="C72" s="4" t="str">
         <f t="shared" ref="C72:C88" si="4">IF(A72="","",CONCATENATE("| ",SUBSTITUTE(A72,"=="," | ")," |"))</f>
         <v/>
       </c>
-      <c r="E72" s="18" t="str">
+      <c r="E72" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="73" spans="3:5">
-      <c r="C73" s="15" t="str">
+      <c r="C73" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E73" s="18" t="str">
+      <c r="E73" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="3:5">
-      <c r="C74" s="15" t="str">
+      <c r="C74" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E74" s="18" t="str">
+      <c r="E74" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="75" spans="3:5">
-      <c r="C75" s="15" t="str">
+      <c r="C75" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E75" s="18" t="str">
+      <c r="E75" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="76" spans="3:5">
-      <c r="C76" s="15" t="str">
+      <c r="C76" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E76" s="18" t="str">
+      <c r="E76" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="3:5">
-      <c r="C77" s="15" t="str">
+      <c r="C77" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E77" s="18" t="str">
+      <c r="E77" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="3:5">
-      <c r="C78" s="15" t="str">
+      <c r="C78" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E78" s="18" t="str">
+      <c r="E78" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="3:5">
-      <c r="C79" s="15" t="str">
+      <c r="C79" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E79" s="18" t="str">
+      <c r="E79" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="3:5">
-      <c r="C80" s="15" t="str">
+      <c r="C80" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E80" s="18" t="str">
+      <c r="E80" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="3:5">
-      <c r="C81" s="15" t="str">
+      <c r="C81" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E81" s="18" t="str">
+      <c r="E81" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="3:5">
-      <c r="C82" s="15" t="str">
+      <c r="C82" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E82" s="18" t="str">
+      <c r="E82" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="3:5">
-      <c r="C83" s="15" t="str">
+      <c r="C83" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E83" s="18" t="str">
+      <c r="E83" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="3:5">
-      <c r="C84" s="15" t="str">
+      <c r="C84" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E84" s="18" t="str">
+      <c r="E84" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="3:5">
-      <c r="C85" s="15" t="str">
+      <c r="C85" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E85" s="18" t="str">
+      <c r="E85" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="3:5">
-      <c r="C86" s="15" t="str">
+      <c r="C86" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E86" s="18" t="str">
+      <c r="E86" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="3:5">
-      <c r="C87" s="15" t="str">
+      <c r="C87" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E87" s="18" t="str">
+      <c r="E87" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="3:5">
-      <c r="C88" s="15" t="str">
+      <c r="C88" s="4" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="E88" s="18" t="str">
+      <c r="E88" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
:ok: Back to the track, and add Flask-SQLAlchemy
</commit_message>
<xml_diff>
--- a/installed_packages_to_markdown.xlsx
+++ b/installed_packages_to_markdown.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Step 1. Run the comand line below.</t>
   </si>
@@ -54,6 +54,9 @@
     <t>Flask==1.0.2</t>
   </si>
   <si>
+    <t>Flask-SQLAlchemy==2.3.2</t>
+  </si>
+  <si>
     <t>Flask-Uploads==0.2.1</t>
   </si>
   <si>
@@ -106,6 +109,9 @@
   </si>
   <si>
     <t>six==1.12.0</t>
+  </si>
+  <si>
+    <t>SQLAlchemy==1.3.0</t>
   </si>
   <si>
     <t>typed-ast==1.3.1</t>
@@ -123,9 +129,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -188,16 +194,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -209,24 +216,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -240,9 +231,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,6 +247,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -265,15 +264,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,7 +302,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -295,41 +331,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -352,13 +358,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,169 +412,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,32 +598,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -649,16 +649,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -672,11 +672,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,130 +691,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -817,16 +823,16 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1233,9 +1239,9 @@
   <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1378,11 +1384,11 @@
       </c>
       <c r="C11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Flask-Uploads | 0.2.1 |</v>
+        <v>| Flask-SQLAlchemy | 2.3.2 |</v>
       </c>
       <c r="E11" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Flask-Uploads,0.2.1</v>
+        <v>Flask-SQLAlchemy,2.3.2</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1391,11 +1397,11 @@
       </c>
       <c r="C12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| isort | 4.3.4 |</v>
+        <v>| Flask-Uploads | 0.2.1 |</v>
       </c>
       <c r="E12" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>isort,4.3.4</v>
+        <v>Flask-Uploads,0.2.1</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1404,11 +1410,11 @@
       </c>
       <c r="C13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| itsdangerous | 1.1.0 |</v>
+        <v>| isort | 4.3.4 |</v>
       </c>
       <c r="E13" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>itsdangerous,1.1.0</v>
+        <v>isort,4.3.4</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1417,11 +1423,11 @@
       </c>
       <c r="C14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| jdcal | 1.4 |</v>
+        <v>| itsdangerous | 1.1.0 |</v>
       </c>
       <c r="E14" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>jdcal,1.4</v>
+        <v>itsdangerous,1.1.0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1430,11 +1436,11 @@
       </c>
       <c r="C15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Jinja2 | 2.10 |</v>
+        <v>| jdcal | 1.4 |</v>
       </c>
       <c r="E15" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Jinja2,2.10</v>
+        <v>jdcal,1.4</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1443,11 +1449,11 @@
       </c>
       <c r="C16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| lazy-object-proxy | 1.3.1 |</v>
+        <v>| Jinja2 | 2.10 |</v>
       </c>
       <c r="E16" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>lazy-object-proxy,1.3.1</v>
+        <v>Jinja2,2.10</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1456,11 +1462,11 @@
       </c>
       <c r="C17" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| lml | 0.0.9 |</v>
+        <v>| lazy-object-proxy | 1.3.1 |</v>
       </c>
       <c r="E17" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>lml,0.0.9</v>
+        <v>lazy-object-proxy,1.3.1</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1469,11 +1475,11 @@
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Markdown | 3.0.1 |</v>
+        <v>| lml | 0.0.9 |</v>
       </c>
       <c r="E18" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Markdown,3.0.1</v>
+        <v>lml,0.0.9</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1482,11 +1488,11 @@
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| MarkupSafe | 1.1.0 |</v>
+        <v>| Markdown | 3.0.1 |</v>
       </c>
       <c r="E19" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>MarkupSafe,1.1.0</v>
+        <v>Markdown,3.0.1</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1495,11 +1501,11 @@
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| mccabe | 0.6.1 |</v>
+        <v>| MarkupSafe | 1.1.0 |</v>
       </c>
       <c r="E20" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>mccabe,0.6.1</v>
+        <v>MarkupSafe,1.1.0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1508,11 +1514,11 @@
       </c>
       <c r="C21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| openpyxl | 2.6.0 |</v>
+        <v>| mccabe | 0.6.1 |</v>
       </c>
       <c r="E21" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>openpyxl,2.6.0</v>
+        <v>mccabe,0.6.1</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1521,11 +1527,11 @@
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pip | 9.0.1 |</v>
+        <v>| openpyxl | 2.6.0 |</v>
       </c>
       <c r="E22" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pip,9.0.1</v>
+        <v>openpyxl,2.6.0</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1534,11 +1540,11 @@
       </c>
       <c r="C23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pkg-resources | 0.0.0 |</v>
+        <v>| pip | 9.0.1 |</v>
       </c>
       <c r="E23" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pkg-resources,0.0.0</v>
+        <v>pip,9.0.1</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1547,11 +1553,11 @@
       </c>
       <c r="C24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pyexcel-io | 0.5.14 |</v>
+        <v>| pkg-resources | 0.0.0 |</v>
       </c>
       <c r="E24" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pyexcel-io,0.5.14</v>
+        <v>pkg-resources,0.0.0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1560,11 +1566,11 @@
       </c>
       <c r="C25" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pyexcel-xlsx | 0.5.7 |</v>
+        <v>| pyexcel-io | 0.5.14 |</v>
       </c>
       <c r="E25" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pyexcel-xlsx,0.5.7</v>
+        <v>pyexcel-io,0.5.14</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1573,11 +1579,11 @@
       </c>
       <c r="C26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pylint | 2.2.2 |</v>
+        <v>| pyexcel-xlsx | 0.5.7 |</v>
       </c>
       <c r="E26" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pylint,2.2.2</v>
+        <v>pyexcel-xlsx,0.5.7</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1586,11 +1592,11 @@
       </c>
       <c r="C27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| setuptools | 40.8.0 |</v>
+        <v>| pylint | 2.2.2 |</v>
       </c>
       <c r="E27" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>setuptools,40.8.0</v>
+        <v>pylint,2.2.2</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1599,11 +1605,11 @@
       </c>
       <c r="C28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| six | 1.12.0 |</v>
+        <v>| setuptools | 40.8.0 |</v>
       </c>
       <c r="E28" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>six,1.12.0</v>
+        <v>setuptools,40.8.0</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1612,11 +1618,11 @@
       </c>
       <c r="C29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| typed-ast | 1.3.1 |</v>
+        <v>| six | 1.12.0 |</v>
       </c>
       <c r="E29" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>typed-ast,1.3.1</v>
+        <v>six,1.12.0</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1625,11 +1631,11 @@
       </c>
       <c r="C30" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Werkzeug | 0.14.1 |</v>
+        <v>| SQLAlchemy | 1.3.0 |</v>
       </c>
       <c r="E30" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Werkzeug,0.14.1</v>
+        <v>SQLAlchemy,1.3.0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1638,31 +1644,37 @@
       </c>
       <c r="C31" s="4" t="str">
         <f t="shared" si="1"/>
+        <v>| typed-ast | 1.3.1 |</v>
+      </c>
+      <c r="E31" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>typed-ast,1.3.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| Werkzeug | 0.14.1 |</v>
+      </c>
+      <c r="E32" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>Werkzeug,0.14.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="4" t="str">
+        <f t="shared" si="1"/>
         <v>| wrapt | 1.11.1 |</v>
       </c>
-      <c r="E31" s="16" t="str">
+      <c r="E33" s="16" t="str">
         <f t="shared" si="0"/>
         <v>wrapt,1.11.1</v>
-      </c>
-    </row>
-    <row r="32" spans="3:5">
-      <c r="C32" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E32" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="3:5">
-      <c r="C33" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E33" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
       </c>
     </row>
     <row r="34" spans="3:5">

</xml_diff>

<commit_message>
Learn about version control :grin:
</commit_message>
<xml_diff>
--- a/installed_packages_to_markdown.xlsx
+++ b/installed_packages_to_markdown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20670" windowHeight="10245"/>
+    <workbookView windowWidth="20175" windowHeight="10245"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Step 1. Run the comand line below.</t>
   </si>
@@ -54,6 +54,9 @@
     <t>Flask==1.0.2</t>
   </si>
   <si>
+    <t>bumpversion==0.5.3</t>
+  </si>
+  <si>
     <t>Flask-SQLAlchemy==2.3.2</t>
   </si>
   <si>
@@ -96,12 +99,24 @@
     <t>pkg-resources==0.0.0</t>
   </si>
   <si>
+    <t>pycodestyle==2.5.0</t>
+  </si>
+  <si>
+    <t>pydocstyle==3.0.0</t>
+  </si>
+  <si>
     <t>pyexcel-io==0.5.14</t>
   </si>
   <si>
     <t>pyexcel-xlsx==0.5.7</t>
   </si>
   <si>
+    <t>pyflakes==2.1.1</t>
+  </si>
+  <si>
+    <t>pylama==7.6.6</t>
+  </si>
+  <si>
     <t>pylint==2.2.2</t>
   </si>
   <si>
@@ -109,6 +124,9 @@
   </si>
   <si>
     <t>six==1.12.0</t>
+  </si>
+  <si>
+    <t>snowballstemmer==1.2.1</t>
   </si>
   <si>
     <t>SQLAlchemy==1.3.0</t>
@@ -129,9 +147,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -195,6 +213,106 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,16 +326,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -225,82 +335,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -309,33 +349,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -358,187 +376,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,6 +626,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -648,30 +681,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -686,153 +695,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1239,9 +1257,9 @@
   <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1380,401 +1398,431 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Flask-SQLAlchemy | 2.3.2 |</v>
+        <v>| astroid | 2.1.0 |</v>
       </c>
       <c r="E11" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Flask-SQLAlchemy,2.3.2</v>
+        <v>astroid,2.1.0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Flask-Uploads | 0.2.1 |</v>
+        <v>| bumpversion | 0.5.3 |</v>
       </c>
       <c r="E12" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Flask-Uploads,0.2.1</v>
+        <v>bumpversion,0.5.3</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| isort | 4.3.4 |</v>
+        <v>| Click | 7.0 |</v>
       </c>
       <c r="E13" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>isort,4.3.4</v>
+        <v>Click,7.0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| itsdangerous | 1.1.0 |</v>
+        <v>| et-xmlfile | 1.0.1 |</v>
       </c>
       <c r="E14" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>itsdangerous,1.1.0</v>
+        <v>et-xmlfile,1.0.1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| jdcal | 1.4 |</v>
+        <v>| Flask | 1.0.2 |</v>
       </c>
       <c r="E15" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>jdcal,1.4</v>
+        <v>Flask,1.0.2</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Jinja2 | 2.10 |</v>
+        <v>| Flask-SQLAlchemy | 2.3.2 |</v>
       </c>
       <c r="E16" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Jinja2,2.10</v>
+        <v>Flask-SQLAlchemy,2.3.2</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C17" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| lazy-object-proxy | 1.3.1 |</v>
+        <v>| Flask-Uploads | 0.2.1 |</v>
       </c>
       <c r="E17" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>lazy-object-proxy,1.3.1</v>
+        <v>Flask-Uploads,0.2.1</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| lml | 0.0.9 |</v>
+        <v>| isort | 4.3.4 |</v>
       </c>
       <c r="E18" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>lml,0.0.9</v>
+        <v>isort,4.3.4</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Markdown | 3.0.1 |</v>
+        <v>| itsdangerous | 1.1.0 |</v>
       </c>
       <c r="E19" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Markdown,3.0.1</v>
+        <v>itsdangerous,1.1.0</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| MarkupSafe | 1.1.0 |</v>
+        <v>| jdcal | 1.4 |</v>
       </c>
       <c r="E20" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>MarkupSafe,1.1.0</v>
+        <v>jdcal,1.4</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| mccabe | 0.6.1 |</v>
+        <v>| Jinja2 | 2.10 |</v>
       </c>
       <c r="E21" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>mccabe,0.6.1</v>
+        <v>Jinja2,2.10</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| openpyxl | 2.6.0 |</v>
+        <v>| lazy-object-proxy | 1.3.1 |</v>
       </c>
       <c r="E22" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>openpyxl,2.6.0</v>
+        <v>lazy-object-proxy,1.3.1</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pip | 9.0.1 |</v>
+        <v>| lml | 0.0.9 |</v>
       </c>
       <c r="E23" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pip,9.0.1</v>
+        <v>lml,0.0.9</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pkg-resources | 0.0.0 |</v>
+        <v>| Markdown | 3.0.1 |</v>
       </c>
       <c r="E24" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pkg-resources,0.0.0</v>
+        <v>Markdown,3.0.1</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C25" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pyexcel-io | 0.5.14 |</v>
+        <v>| MarkupSafe | 1.1.0 |</v>
       </c>
       <c r="E25" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pyexcel-io,0.5.14</v>
+        <v>MarkupSafe,1.1.0</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pyexcel-xlsx | 0.5.7 |</v>
+        <v>| mccabe | 0.6.1 |</v>
       </c>
       <c r="E26" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pyexcel-xlsx,0.5.7</v>
+        <v>mccabe,0.6.1</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pylint | 2.2.2 |</v>
+        <v>| openpyxl | 2.6.0 |</v>
       </c>
       <c r="E27" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pylint,2.2.2</v>
+        <v>openpyxl,2.6.0</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| setuptools | 40.8.0 |</v>
+        <v>| pip | 9.0.1 |</v>
       </c>
       <c r="E28" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>setuptools,40.8.0</v>
+        <v>pip,9.0.1</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| six | 1.12.0 |</v>
+        <v>| pkg-resources | 0.0.0 |</v>
       </c>
       <c r="E29" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>six,1.12.0</v>
+        <v>pkg-resources,0.0.0</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C30" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| SQLAlchemy | 1.3.0 |</v>
+        <v>| pycodestyle | 2.5.0 |</v>
       </c>
       <c r="E30" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>SQLAlchemy,1.3.0</v>
+        <v>pycodestyle,2.5.0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C31" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| typed-ast | 1.3.1 |</v>
+        <v>| pydocstyle | 3.0.0 |</v>
       </c>
       <c r="E31" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>typed-ast,1.3.1</v>
+        <v>pydocstyle,3.0.0</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C32" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Werkzeug | 0.14.1 |</v>
+        <v>| pyexcel-io | 0.5.14 |</v>
       </c>
       <c r="E32" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Werkzeug,0.14.1</v>
+        <v>pyexcel-io,0.5.14</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| pyexcel-xlsx | 0.5.7 |</v>
+      </c>
+      <c r="E33" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>pyexcel-xlsx,0.5.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| pyflakes | 2.1.1 |</v>
+      </c>
+      <c r="E34" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>pyflakes,2.1.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| pylama | 7.6.6 |</v>
+      </c>
+      <c r="E35" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>pylama,7.6.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| pylint | 2.2.2 |</v>
+      </c>
+      <c r="E36" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>pylint,2.2.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>| wrapt | 1.11.1 |</v>
-      </c>
-      <c r="E33" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>wrapt,1.11.1</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5">
-      <c r="C34" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E34" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="3:5">
-      <c r="C35" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E35" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="3:5">
-      <c r="C36" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E36" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="3:5">
       <c r="C37" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>| setuptools | 40.8.0 |</v>
       </c>
       <c r="E37" s="16" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="3:5">
+        <v>setuptools,40.8.0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C38" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>| six | 1.12.0 |</v>
       </c>
       <c r="E38" s="16" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="3:5">
+        <v>six,1.12.0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C39" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>| snowballstemmer | 1.2.1 |</v>
       </c>
       <c r="E39" s="16" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="3:5">
+        <v>snowballstemmer,1.2.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C40" s="4" t="str">
         <f t="shared" ref="C40:C71" si="2">IF(A40="","",CONCATENATE("| ",SUBSTITUTE(A40,"=="," | ")," |"))</f>
-        <v/>
+        <v>| SQLAlchemy | 1.3.0 |</v>
       </c>
       <c r="E40" s="16" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="3:5">
+        <v>SQLAlchemy,1.3.0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C41" s="4" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>| typed-ast | 1.3.1 |</v>
       </c>
       <c r="E41" s="16" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="3:5">
+        <v>typed-ast,1.3.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C42" s="4" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>| Werkzeug | 0.14.1 |</v>
       </c>
       <c r="E42" s="16" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="3:5">
+        <v>Werkzeug,0.14.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C43" s="4" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>| wrapt | 1.11.1 |</v>
       </c>
       <c r="E43" s="16" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>wrapt,1.11.1</v>
       </c>
     </row>
     <row r="44" spans="3:5">

</xml_diff>

<commit_message>
Update README And Reset venv on Ubuntu 19.04 ⬆
</commit_message>
<xml_diff>
--- a/installed_packages_to_markdown.xlsx
+++ b/installed_packages_to_markdown.xlsx
@@ -4,19 +4,17 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20175" windowHeight="10245"/>
+    <workbookView windowWidth="20175" windowHeight="9795"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="20190721" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Step 1. Run the comand line below.</t>
   </si>
@@ -42,103 +40,58 @@
     <t>"-----","-----"</t>
   </si>
   <si>
-    <t>astroid==2.1.0</t>
-  </si>
-  <si>
     <t>Click==7.0</t>
   </si>
   <si>
     <t>et-xmlfile==1.0.1</t>
   </si>
   <si>
-    <t>Flask==1.0.2</t>
-  </si>
-  <si>
-    <t>bumpversion==0.5.3</t>
-  </si>
-  <si>
-    <t>Flask-SQLAlchemy==2.3.2</t>
+    <t>Flask==1.1.1</t>
   </si>
   <si>
     <t>Flask-Uploads==0.2.1</t>
   </si>
   <si>
-    <t>isort==4.3.4</t>
-  </si>
-  <si>
     <t>itsdangerous==1.1.0</t>
   </si>
   <si>
-    <t>jdcal==1.4</t>
-  </si>
-  <si>
-    <t>Jinja2==2.10</t>
-  </si>
-  <si>
-    <t>lazy-object-proxy==1.3.1</t>
+    <t>jdcal==1.4.1</t>
+  </si>
+  <si>
+    <t>Jinja2==2.10.1</t>
   </si>
   <si>
     <t>lml==0.0.9</t>
   </si>
   <si>
-    <t>Markdown==3.0.1</t>
-  </si>
-  <si>
-    <t>MarkupSafe==1.1.0</t>
-  </si>
-  <si>
-    <t>mccabe==0.6.1</t>
-  </si>
-  <si>
-    <t>openpyxl==2.6.0</t>
-  </si>
-  <si>
-    <t>pip==9.0.1</t>
+    <t>Markdown==3.1.1</t>
+  </si>
+  <si>
+    <t>MarkupSafe==1.1.1</t>
+  </si>
+  <si>
+    <t>openpyxl==2.5.14</t>
+  </si>
+  <si>
+    <t>pip==18.1</t>
   </si>
   <si>
     <t>pkg-resources==0.0.0</t>
   </si>
   <si>
-    <t>pycodestyle==2.5.0</t>
-  </si>
-  <si>
-    <t>pydocstyle==3.0.0</t>
-  </si>
-  <si>
-    <t>pyexcel-io==0.5.14</t>
+    <t>pyexcel-io==0.5.20</t>
   </si>
   <si>
     <t>pyexcel-xlsx==0.5.7</t>
   </si>
   <si>
-    <t>pyflakes==2.1.1</t>
-  </si>
-  <si>
-    <t>pylama==7.6.6</t>
-  </si>
-  <si>
-    <t>pylint==2.2.2</t>
-  </si>
-  <si>
     <t>setuptools==40.8.0</t>
   </si>
   <si>
-    <t>six==1.12.0</t>
-  </si>
-  <si>
-    <t>snowballstemmer==1.2.1</t>
-  </si>
-  <si>
-    <t>SQLAlchemy==1.3.0</t>
-  </si>
-  <si>
-    <t>typed-ast==1.3.1</t>
-  </si>
-  <si>
-    <t>Werkzeug==0.14.1</t>
-  </si>
-  <si>
-    <t>wrapt==1.11.1</t>
+    <t>SQLAlchemy==1.3.5</t>
+  </si>
+  <si>
+    <t>Werkzeug==0.15.5</t>
   </si>
 </sst>
 </file>
@@ -146,9 +99,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
@@ -211,8 +164,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,39 +180,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -272,6 +210,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -281,38 +235,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -335,6 +266,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -349,6 +288,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -376,31 +329,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -412,13 +455,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,19 +479,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,109 +497,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,45 +569,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -677,6 +591,36 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -704,153 +648,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -972,7 +925,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="3D3D3D"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1259,10 +1212,10 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="26.125" style="2" customWidth="1"/>
     <col min="2" max="2" width="1.125" style="3" customWidth="1"/>
@@ -1350,11 +1303,11 @@
       </c>
       <c r="C7" s="4" t="str">
         <f>IF(A7="","",CONCATENATE("| ",SUBSTITUTE(A7,"=="," | ")," |"))</f>
-        <v>| astroid | 2.1.0 |</v>
+        <v>| Click | 7.0 |</v>
       </c>
       <c r="E7" s="16" t="str">
         <f t="shared" ref="E7:E70" si="0">IF(C7="","",SUBSTITUTE(MID(C7,3,LEN(C7)-4)," | ",","))</f>
-        <v>astroid,2.1.0</v>
+        <v>Click,7.0</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1363,11 +1316,11 @@
       </c>
       <c r="C8" s="4" t="str">
         <f t="shared" ref="C8:C39" si="1">IF(A8="","",CONCATENATE("| ",SUBSTITUTE(A8,"=="," | ")," |"))</f>
-        <v>| Click | 7.0 |</v>
+        <v>| et-xmlfile | 1.0.1 |</v>
       </c>
       <c r="E8" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Click,7.0</v>
+        <v>et-xmlfile,1.0.1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1376,11 +1329,11 @@
       </c>
       <c r="C9" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| et-xmlfile | 1.0.1 |</v>
+        <v>| Flask | 1.1.1 |</v>
       </c>
       <c r="E9" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>et-xmlfile,1.0.1</v>
+        <v>Flask,1.1.1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1389,440 +1342,383 @@
       </c>
       <c r="C10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Flask | 1.0.2 |</v>
+        <v>| Flask-Uploads | 0.2.1 |</v>
       </c>
       <c r="E10" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Flask,1.0.2</v>
+        <v>Flask-Uploads,0.2.1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| astroid | 2.1.0 |</v>
+        <v>| itsdangerous | 1.1.0 |</v>
       </c>
       <c r="E11" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>astroid,2.1.0</v>
+        <v>itsdangerous,1.1.0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| bumpversion | 0.5.3 |</v>
+        <v>| jdcal | 1.4.1 |</v>
       </c>
       <c r="E12" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>bumpversion,0.5.3</v>
+        <v>jdcal,1.4.1</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Click | 7.0 |</v>
+        <v>| Jinja2 | 2.10.1 |</v>
       </c>
       <c r="E13" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Click,7.0</v>
+        <v>Jinja2,2.10.1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| et-xmlfile | 1.0.1 |</v>
+        <v>| lml | 0.0.9 |</v>
       </c>
       <c r="E14" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>et-xmlfile,1.0.1</v>
+        <v>lml,0.0.9</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Flask | 1.0.2 |</v>
+        <v>| Markdown | 3.1.1 |</v>
       </c>
       <c r="E15" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Flask,1.0.2</v>
+        <v>Markdown,3.1.1</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Flask-SQLAlchemy | 2.3.2 |</v>
+        <v>| MarkupSafe | 1.1.1 |</v>
       </c>
       <c r="E16" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Flask-SQLAlchemy,2.3.2</v>
+        <v>MarkupSafe,1.1.1</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C17" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Flask-Uploads | 0.2.1 |</v>
+        <v>| openpyxl | 2.5.14 |</v>
       </c>
       <c r="E17" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Flask-Uploads,0.2.1</v>
+        <v>openpyxl,2.5.14</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| isort | 4.3.4 |</v>
+        <v>| pip | 18.1 |</v>
       </c>
       <c r="E18" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>isort,4.3.4</v>
+        <v>pip,18.1</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| itsdangerous | 1.1.0 |</v>
+        <v>| pkg-resources | 0.0.0 |</v>
       </c>
       <c r="E19" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>itsdangerous,1.1.0</v>
+        <v>pkg-resources,0.0.0</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| jdcal | 1.4 |</v>
+        <v>| pyexcel-io | 0.5.20 |</v>
       </c>
       <c r="E20" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>jdcal,1.4</v>
+        <v>pyexcel-io,0.5.20</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Jinja2 | 2.10 |</v>
+        <v>| pyexcel-xlsx | 0.5.7 |</v>
       </c>
       <c r="E21" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Jinja2,2.10</v>
+        <v>pyexcel-xlsx,0.5.7</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| lazy-object-proxy | 1.3.1 |</v>
+        <v>| setuptools | 40.8.0 |</v>
       </c>
       <c r="E22" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>lazy-object-proxy,1.3.1</v>
+        <v>setuptools,40.8.0</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| lml | 0.0.9 |</v>
+        <v>| SQLAlchemy | 1.3.5 |</v>
       </c>
       <c r="E23" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>lml,0.0.9</v>
+        <v>SQLAlchemy,1.3.5</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Markdown | 3.0.1 |</v>
+        <v>| Werkzeug | 0.15.5 |</v>
       </c>
       <c r="E24" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Markdown,3.0.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>Werkzeug,0.15.5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5">
       <c r="C25" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| MarkupSafe | 1.1.0 |</v>
+        <v/>
       </c>
       <c r="E25" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>MarkupSafe,1.1.0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="3:5">
       <c r="C26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| mccabe | 0.6.1 |</v>
+        <v/>
       </c>
       <c r="E26" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>mccabe,0.6.1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="3:5">
       <c r="C27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| openpyxl | 2.6.0 |</v>
+        <v/>
       </c>
       <c r="E27" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>openpyxl,2.6.0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="3:5">
       <c r="C28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pip | 9.0.1 |</v>
+        <v/>
       </c>
       <c r="E28" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pip,9.0.1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="3:5">
       <c r="C29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pkg-resources | 0.0.0 |</v>
+        <v/>
       </c>
       <c r="E29" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pkg-resources,0.0.0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="3:5">
       <c r="C30" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pycodestyle | 2.5.0 |</v>
+        <v/>
       </c>
       <c r="E30" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pycodestyle,2.5.0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="3:5">
       <c r="C31" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pydocstyle | 3.0.0 |</v>
+        <v/>
       </c>
       <c r="E31" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pydocstyle,3.0.0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="3:5">
       <c r="C32" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pyexcel-io | 0.5.14 |</v>
+        <v/>
       </c>
       <c r="E32" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pyexcel-io,0.5.14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="3:5">
       <c r="C33" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pyexcel-xlsx | 0.5.7 |</v>
+        <v/>
       </c>
       <c r="E33" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pyexcel-xlsx,0.5.7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="3:5">
       <c r="C34" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pyflakes | 2.1.1 |</v>
+        <v/>
       </c>
       <c r="E34" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pyflakes,2.1.1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="3:5">
       <c r="C35" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pylama | 7.6.6 |</v>
+        <v/>
       </c>
       <c r="E35" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pylama,7.6.6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="3:5">
       <c r="C36" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pylint | 2.2.2 |</v>
+        <v/>
       </c>
       <c r="E36" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pylint,2.2.2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="3:5">
       <c r="C37" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| setuptools | 40.8.0 |</v>
+        <v/>
       </c>
       <c r="E37" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>setuptools,40.8.0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="3:5">
       <c r="C38" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| six | 1.12.0 |</v>
+        <v/>
       </c>
       <c r="E38" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>six,1.12.0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="3:5">
       <c r="C39" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| snowballstemmer | 1.2.1 |</v>
+        <v/>
       </c>
       <c r="E39" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>snowballstemmer,1.2.1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="3:5">
       <c r="C40" s="4" t="str">
         <f t="shared" ref="C40:C71" si="2">IF(A40="","",CONCATENATE("| ",SUBSTITUTE(A40,"=="," | ")," |"))</f>
-        <v>| SQLAlchemy | 1.3.0 |</v>
+        <v/>
       </c>
       <c r="E40" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>SQLAlchemy,1.3.0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="3:5">
       <c r="C41" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>| typed-ast | 1.3.1 |</v>
+        <v/>
       </c>
       <c r="E41" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>typed-ast,1.3.1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="3:5">
       <c r="C42" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>| Werkzeug | 0.14.1 |</v>
+        <v/>
       </c>
       <c r="E42" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Werkzeug,0.14.1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="3:5">
       <c r="C43" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>| wrapt | 1.11.1 |</v>
+        <v/>
       </c>
       <c r="E43" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>wrapt,1.11.1</v>
+        <v/>
       </c>
     </row>
     <row r="44" spans="3:5">
@@ -2286,38 +2182,4 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Blog update #20190721 💬
</commit_message>
<xml_diff>
--- a/installed_packages_to_markdown.xlsx
+++ b/installed_packages_to_markdown.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Step 1. Run the comand line below.</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>"-----","-----"</t>
+  </si>
+  <si>
+    <t>bumpversion==0.5.3</t>
   </si>
   <si>
     <t>Click==7.0</t>
@@ -99,10 +102,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -162,14 +165,6 @@
       <color theme="9" tint="-0.5"/>
       <name val="Microsoft YaHei"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -180,23 +175,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,6 +215,37 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -227,23 +253,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -258,13 +275,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -274,21 +290,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -300,13 +310,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -329,43 +332,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,13 +446,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -395,115 +506,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,6 +572,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -580,17 +622,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -610,36 +641,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -651,9 +652,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -662,148 +665,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1212,7 +1215,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="7"/>
@@ -1303,11 +1306,11 @@
       </c>
       <c r="C7" s="4" t="str">
         <f>IF(A7="","",CONCATENATE("| ",SUBSTITUTE(A7,"=="," | ")," |"))</f>
-        <v>| Click | 7.0 |</v>
+        <v>| bumpversion | 0.5.3 |</v>
       </c>
       <c r="E7" s="16" t="str">
         <f t="shared" ref="E7:E70" si="0">IF(C7="","",SUBSTITUTE(MID(C7,3,LEN(C7)-4)," | ",","))</f>
-        <v>Click,7.0</v>
+        <v>bumpversion,0.5.3</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1316,11 +1319,11 @@
       </c>
       <c r="C8" s="4" t="str">
         <f t="shared" ref="C8:C39" si="1">IF(A8="","",CONCATENATE("| ",SUBSTITUTE(A8,"=="," | ")," |"))</f>
-        <v>| et-xmlfile | 1.0.1 |</v>
+        <v>| Click | 7.0 |</v>
       </c>
       <c r="E8" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>et-xmlfile,1.0.1</v>
+        <v>Click,7.0</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1329,11 +1332,11 @@
       </c>
       <c r="C9" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Flask | 1.1.1 |</v>
+        <v>| et-xmlfile | 1.0.1 |</v>
       </c>
       <c r="E9" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Flask,1.1.1</v>
+        <v>et-xmlfile,1.0.1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1342,11 +1345,11 @@
       </c>
       <c r="C10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Flask-Uploads | 0.2.1 |</v>
+        <v>| Flask | 1.1.1 |</v>
       </c>
       <c r="E10" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Flask-Uploads,0.2.1</v>
+        <v>Flask,1.1.1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1355,11 +1358,11 @@
       </c>
       <c r="C11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| itsdangerous | 1.1.0 |</v>
+        <v>| Flask-Uploads | 0.2.1 |</v>
       </c>
       <c r="E11" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>itsdangerous,1.1.0</v>
+        <v>Flask-Uploads,0.2.1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1368,11 +1371,11 @@
       </c>
       <c r="C12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| jdcal | 1.4.1 |</v>
+        <v>| itsdangerous | 1.1.0 |</v>
       </c>
       <c r="E12" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>jdcal,1.4.1</v>
+        <v>itsdangerous,1.1.0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1381,11 +1384,11 @@
       </c>
       <c r="C13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Jinja2 | 2.10.1 |</v>
+        <v>| jdcal | 1.4.1 |</v>
       </c>
       <c r="E13" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Jinja2,2.10.1</v>
+        <v>jdcal,1.4.1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1394,11 +1397,11 @@
       </c>
       <c r="C14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| lml | 0.0.9 |</v>
+        <v>| Jinja2 | 2.10.1 |</v>
       </c>
       <c r="E14" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>lml,0.0.9</v>
+        <v>Jinja2,2.10.1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1407,11 +1410,11 @@
       </c>
       <c r="C15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Markdown | 3.1.1 |</v>
+        <v>| lml | 0.0.9 |</v>
       </c>
       <c r="E15" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Markdown,3.1.1</v>
+        <v>lml,0.0.9</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1420,11 +1423,11 @@
       </c>
       <c r="C16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| MarkupSafe | 1.1.1 |</v>
+        <v>| Markdown | 3.1.1 |</v>
       </c>
       <c r="E16" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>MarkupSafe,1.1.1</v>
+        <v>Markdown,3.1.1</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1433,11 +1436,11 @@
       </c>
       <c r="C17" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| openpyxl | 2.5.14 |</v>
+        <v>| MarkupSafe | 1.1.1 |</v>
       </c>
       <c r="E17" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>openpyxl,2.5.14</v>
+        <v>MarkupSafe,1.1.1</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1446,11 +1449,11 @@
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pip | 18.1 |</v>
+        <v>| openpyxl | 2.5.14 |</v>
       </c>
       <c r="E18" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pip,18.1</v>
+        <v>openpyxl,2.5.14</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1459,11 +1462,11 @@
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pkg-resources | 0.0.0 |</v>
+        <v>| pip | 18.1 |</v>
       </c>
       <c r="E19" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pkg-resources,0.0.0</v>
+        <v>pip,18.1</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1472,11 +1475,11 @@
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pyexcel-io | 0.5.20 |</v>
+        <v>| pkg-resources | 0.0.0 |</v>
       </c>
       <c r="E20" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pyexcel-io,0.5.20</v>
+        <v>pkg-resources,0.0.0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1485,11 +1488,11 @@
       </c>
       <c r="C21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pyexcel-xlsx | 0.5.7 |</v>
+        <v>| pyexcel-io | 0.5.20 |</v>
       </c>
       <c r="E21" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pyexcel-xlsx,0.5.7</v>
+        <v>pyexcel-io,0.5.20</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1498,11 +1501,11 @@
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| setuptools | 40.8.0 |</v>
+        <v>| pyexcel-xlsx | 0.5.7 |</v>
       </c>
       <c r="E22" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>setuptools,40.8.0</v>
+        <v>pyexcel-xlsx,0.5.7</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1511,11 +1514,11 @@
       </c>
       <c r="C23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| SQLAlchemy | 1.3.5 |</v>
+        <v>| setuptools | 40.8.0 |</v>
       </c>
       <c r="E23" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>SQLAlchemy,1.3.5</v>
+        <v>setuptools,40.8.0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1524,21 +1527,24 @@
       </c>
       <c r="C24" s="4" t="str">
         <f t="shared" si="1"/>
+        <v>| SQLAlchemy | 1.3.5 |</v>
+      </c>
+      <c r="E24" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>SQLAlchemy,1.3.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="4" t="str">
+        <f t="shared" si="1"/>
         <v>| Werkzeug | 0.15.5 |</v>
       </c>
-      <c r="E24" s="16" t="str">
+      <c r="E25" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Werkzeug,0.15.5</v>
-      </c>
-    </row>
-    <row r="25" spans="3:5">
-      <c r="C25" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E25" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
       </c>
     </row>
     <row r="26" spans="3:5">

</xml_diff>

<commit_message>
Update installed_packages.txt and README.md 🍢
</commit_message>
<xml_diff>
--- a/installed_packages_to_markdown.xlsx
+++ b/installed_packages_to_markdown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20175" windowHeight="9795"/>
+    <workbookView windowWidth="19965" windowHeight="9900"/>
   </bookViews>
   <sheets>
     <sheet name="20190721" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Step 1. Run the comand line below.</t>
   </si>
   <si>
-    <t>pip list -l --format=freeze &gt; installed_packages.txt</t>
+    <r>
+      <t>pip</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>list</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>-l</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>--format=freeze</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Microsoft YaHei"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>installed_packages.txt</t>
+    </r>
   </si>
   <si>
     <t>Step 2. Open the txt file, then copy and paste the content to the cells of the column A below.</t>
@@ -40,6 +142,9 @@
     <t>"-----","-----"</t>
   </si>
   <si>
+    <t>astroid==2.3.1</t>
+  </si>
+  <si>
     <t>bumpversion==0.5.3</t>
   </si>
   <si>
@@ -55,6 +160,9 @@
     <t>Flask-Uploads==0.2.1</t>
   </si>
   <si>
+    <t>isort==4.3.21</t>
+  </si>
+  <si>
     <t>itsdangerous==1.1.0</t>
   </si>
   <si>
@@ -64,6 +172,9 @@
     <t>Jinja2==2.10.1</t>
   </si>
   <si>
+    <t>lazy-object-proxy==1.4.2</t>
+  </si>
+  <si>
     <t>lml==0.0.9</t>
   </si>
   <si>
@@ -73,6 +184,9 @@
     <t>MarkupSafe==1.1.1</t>
   </si>
   <si>
+    <t>mccabe==0.6.1</t>
+  </si>
+  <si>
     <t>openpyxl==2.5.14</t>
   </si>
   <si>
@@ -82,19 +196,46 @@
     <t>pkg-resources==0.0.0</t>
   </si>
   <si>
+    <t>pycodestyle==2.5.0</t>
+  </si>
+  <si>
+    <t>pydocstyle==4.0.0</t>
+  </si>
+  <si>
     <t>pyexcel-io==0.5.20</t>
   </si>
   <si>
     <t>pyexcel-xlsx==0.5.7</t>
   </si>
   <si>
+    <t>pyflakes==2.1.1</t>
+  </si>
+  <si>
+    <t>pylama==7.7.1</t>
+  </si>
+  <si>
+    <t>pylint==2.4.2</t>
+  </si>
+  <si>
     <t>setuptools==40.8.0</t>
   </si>
   <si>
+    <t>six==1.12.0</t>
+  </si>
+  <si>
+    <t>snowballstemmer==1.9.0</t>
+  </si>
+  <si>
     <t>SQLAlchemy==1.3.5</t>
   </si>
   <si>
+    <t>typed-ast==1.4.0</t>
+  </si>
+  <si>
     <t>Werkzeug==0.15.5</t>
+  </si>
+  <si>
+    <t>wrapt==1.11.2</t>
   </si>
 </sst>
 </file>
@@ -102,16 +243,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -131,6 +272,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
       <name val="Microsoft YaHei"/>
       <charset val="134"/>
     </font>
@@ -167,149 +315,149 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -332,37 +480,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,66 +654,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -441,78 +661,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -566,23 +714,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -596,17 +729,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -641,11 +768,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -665,148 +813,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -838,81 +986,81 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1215,7 +1363,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="7"/>
@@ -1306,11 +1454,11 @@
       </c>
       <c r="C7" s="4" t="str">
         <f>IF(A7="","",CONCATENATE("| ",SUBSTITUTE(A7,"=="," | ")," |"))</f>
-        <v>| bumpversion | 0.5.3 |</v>
+        <v>| astroid | 2.3.1 |</v>
       </c>
       <c r="E7" s="16" t="str">
         <f t="shared" ref="E7:E70" si="0">IF(C7="","",SUBSTITUTE(MID(C7,3,LEN(C7)-4)," | ",","))</f>
-        <v>bumpversion,0.5.3</v>
+        <v>astroid,2.3.1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1319,11 +1467,11 @@
       </c>
       <c r="C8" s="4" t="str">
         <f t="shared" ref="C8:C39" si="1">IF(A8="","",CONCATENATE("| ",SUBSTITUTE(A8,"=="," | ")," |"))</f>
-        <v>| Click | 7.0 |</v>
+        <v>| bumpversion | 0.5.3 |</v>
       </c>
       <c r="E8" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Click,7.0</v>
+        <v>bumpversion,0.5.3</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1332,11 +1480,11 @@
       </c>
       <c r="C9" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| et-xmlfile | 1.0.1 |</v>
+        <v>| Click | 7.0 |</v>
       </c>
       <c r="E9" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>et-xmlfile,1.0.1</v>
+        <v>Click,7.0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1345,11 +1493,11 @@
       </c>
       <c r="C10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Flask | 1.1.1 |</v>
+        <v>| et-xmlfile | 1.0.1 |</v>
       </c>
       <c r="E10" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Flask,1.1.1</v>
+        <v>et-xmlfile,1.0.1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1358,11 +1506,11 @@
       </c>
       <c r="C11" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Flask-Uploads | 0.2.1 |</v>
+        <v>| Flask | 1.1.1 |</v>
       </c>
       <c r="E11" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Flask-Uploads,0.2.1</v>
+        <v>Flask,1.1.1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1371,11 +1519,11 @@
       </c>
       <c r="C12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| itsdangerous | 1.1.0 |</v>
+        <v>| Flask-Uploads | 0.2.1 |</v>
       </c>
       <c r="E12" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>itsdangerous,1.1.0</v>
+        <v>Flask-Uploads,0.2.1</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1384,11 +1532,11 @@
       </c>
       <c r="C13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| jdcal | 1.4.1 |</v>
+        <v>| isort | 4.3.21 |</v>
       </c>
       <c r="E13" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>jdcal,1.4.1</v>
+        <v>isort,4.3.21</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1397,11 +1545,11 @@
       </c>
       <c r="C14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Jinja2 | 2.10.1 |</v>
+        <v>| itsdangerous | 1.1.0 |</v>
       </c>
       <c r="E14" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Jinja2,2.10.1</v>
+        <v>itsdangerous,1.1.0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1410,11 +1558,11 @@
       </c>
       <c r="C15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| lml | 0.0.9 |</v>
+        <v>| jdcal | 1.4.1 |</v>
       </c>
       <c r="E15" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>lml,0.0.9</v>
+        <v>jdcal,1.4.1</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1423,11 +1571,11 @@
       </c>
       <c r="C16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| Markdown | 3.1.1 |</v>
+        <v>| Jinja2 | 2.10.1 |</v>
       </c>
       <c r="E16" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>Markdown,3.1.1</v>
+        <v>Jinja2,2.10.1</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1436,11 +1584,11 @@
       </c>
       <c r="C17" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| MarkupSafe | 1.1.1 |</v>
+        <v>| lazy-object-proxy | 1.4.2 |</v>
       </c>
       <c r="E17" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>MarkupSafe,1.1.1</v>
+        <v>lazy-object-proxy,1.4.2</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1449,11 +1597,11 @@
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| openpyxl | 2.5.14 |</v>
+        <v>| lml | 0.0.9 |</v>
       </c>
       <c r="E18" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>openpyxl,2.5.14</v>
+        <v>lml,0.0.9</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1462,11 +1610,11 @@
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pip | 18.1 |</v>
+        <v>| Markdown | 3.1.1 |</v>
       </c>
       <c r="E19" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pip,18.1</v>
+        <v>Markdown,3.1.1</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1475,11 +1623,11 @@
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pkg-resources | 0.0.0 |</v>
+        <v>| MarkupSafe | 1.1.1 |</v>
       </c>
       <c r="E20" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pkg-resources,0.0.0</v>
+        <v>MarkupSafe,1.1.1</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1488,11 +1636,11 @@
       </c>
       <c r="C21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pyexcel-io | 0.5.20 |</v>
+        <v>| mccabe | 0.6.1 |</v>
       </c>
       <c r="E21" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pyexcel-io,0.5.20</v>
+        <v>mccabe,0.6.1</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1501,11 +1649,11 @@
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| pyexcel-xlsx | 0.5.7 |</v>
+        <v>| openpyxl | 2.5.14 |</v>
       </c>
       <c r="E22" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>pyexcel-xlsx,0.5.7</v>
+        <v>openpyxl,2.5.14</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1514,11 +1662,11 @@
       </c>
       <c r="C23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| setuptools | 40.8.0 |</v>
+        <v>| pip | 18.1 |</v>
       </c>
       <c r="E23" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>setuptools,40.8.0</v>
+        <v>pip,18.1</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1527,11 +1675,11 @@
       </c>
       <c r="C24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>| SQLAlchemy | 1.3.5 |</v>
+        <v>| pkg-resources | 0.0.0 |</v>
       </c>
       <c r="E24" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>SQLAlchemy,1.3.5</v>
+        <v>pkg-resources,0.0.0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1540,141 +1688,180 @@
       </c>
       <c r="C25" s="4" t="str">
         <f t="shared" si="1"/>
+        <v>| pycodestyle | 2.5.0 |</v>
+      </c>
+      <c r="E25" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>pycodestyle,2.5.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| pydocstyle | 4.0.0 |</v>
+      </c>
+      <c r="E26" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>pydocstyle,4.0.0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| pyexcel-io | 0.5.20 |</v>
+      </c>
+      <c r="E27" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>pyexcel-io,0.5.20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| pyexcel-xlsx | 0.5.7 |</v>
+      </c>
+      <c r="E28" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>pyexcel-xlsx,0.5.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| pyflakes | 2.1.1 |</v>
+      </c>
+      <c r="E29" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>pyflakes,2.1.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| pylama | 7.7.1 |</v>
+      </c>
+      <c r="E30" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>pylama,7.7.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| pylint | 2.4.2 |</v>
+      </c>
+      <c r="E31" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>pylint,2.4.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| setuptools | 40.8.0 |</v>
+      </c>
+      <c r="E32" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>setuptools,40.8.0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| six | 1.12.0 |</v>
+      </c>
+      <c r="E33" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>six,1.12.0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| snowballstemmer | 1.9.0 |</v>
+      </c>
+      <c r="E34" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>snowballstemmer,1.9.0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| SQLAlchemy | 1.3.5 |</v>
+      </c>
+      <c r="E35" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>SQLAlchemy,1.3.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>| typed-ast | 1.4.0 |</v>
+      </c>
+      <c r="E36" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>typed-ast,1.4.0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="4" t="str">
+        <f t="shared" si="1"/>
         <v>| Werkzeug | 0.15.5 |</v>
       </c>
-      <c r="E25" s="16" t="str">
+      <c r="E37" s="16" t="str">
         <f t="shared" si="0"/>
         <v>Werkzeug,0.15.5</v>
       </c>
     </row>
-    <row r="26" spans="3:5">
-      <c r="C26" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E26" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="3:5">
-      <c r="C27" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E27" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="3:5">
-      <c r="C28" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E28" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="3:5">
-      <c r="C29" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E29" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="3:5">
-      <c r="C30" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E30" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="3:5">
-      <c r="C31" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E31" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="3:5">
-      <c r="C32" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E32" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="3:5">
-      <c r="C33" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E33" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="3:5">
-      <c r="C34" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E34" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="3:5">
-      <c r="C35" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E35" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="3:5">
-      <c r="C36" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E36" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="3:5">
-      <c r="C37" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E37" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="3:5">
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C38" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>| wrapt | 1.11.2 |</v>
       </c>
       <c r="E38" s="16" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>wrapt,1.11.2</v>
       </c>
     </row>
     <row r="39" spans="3:5">

</xml_diff>